<commit_message>
Fine tuning with 1K rephrased data and Dashboard for feedback display completed
</commit_message>
<xml_diff>
--- a/sfsu-csc-help/frontend/src/components/pages/api/openai_dataset.xlsx
+++ b/sfsu-csc-help/frontend/src/components/pages/api/openai_dataset.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20390"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20391"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Prathiba\890\CSC890-03-Fa22-Team02\sfsu-csc-help\frontend\src\components\pages\api\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B33EFC97-A4BD-41EC-973B-59515FE2DB4F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10B335B9-F297-4F46-8D8D-CDC1F4FAD0A4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="4070" xr2:uid="{88B1889F-2286-4489-8AA3-1453B7AD078B}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="14380" windowHeight="4070" xr2:uid="{88B1889F-2286-4489-8AA3-1453B7AD078B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -619,14 +619,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8859EB52-92E0-4AF6-B86F-BB32B7589C00}">
   <dimension ref="A1:B35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="116.81640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="168.08984375" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.81640625" style="4" customWidth="1"/>
     <col min="3" max="16384" width="8.7265625" style="2"/>
   </cols>
   <sheetData>

</xml_diff>